<commit_message>
Add in additional sequenced data and modify plots
</commit_message>
<xml_diff>
--- a/data/metadata/CN19S_Taxa_Categories.xlsx
+++ b/data/metadata/CN19S_Taxa_Categories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kpitz/github/MBARI-BOG/CN19S_12S/data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F8B028-C84C-4342-BDD8-BF045E906F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FA2C85-FA0C-9B4F-9D93-C6C621C3070E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="25360" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9720" yWindow="2320" windowWidth="25360" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CN19S_Taxa_Categories" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="310">
   <si>
     <t>Kingdom</t>
   </si>
@@ -926,6 +926,30 @@
   </si>
   <si>
     <t>herrings, shads, sardines, hilsa, and menhadens</t>
+  </si>
+  <si>
+    <t>Coryphaenidae</t>
+  </si>
+  <si>
+    <t>Coryphaena</t>
+  </si>
+  <si>
+    <t>Coryphaena hippurus</t>
+  </si>
+  <si>
+    <t>mahi mahi</t>
+  </si>
+  <si>
+    <t>Anoplopomatidae</t>
+  </si>
+  <si>
+    <t>Anoplopoma</t>
+  </si>
+  <si>
+    <t>Anoplopoma fimbria</t>
+  </si>
+  <si>
+    <t>Sablefish</t>
   </si>
 </sst>
 </file>
@@ -1068,7 +1092,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1254,6 +1278,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1415,9 +1445,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1773,10 +1804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1964,31 +1995,29 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F7" t="s">
-        <v>137</v>
-      </c>
-      <c r="G7" t="s">
-        <v>138</v>
-      </c>
-      <c r="H7" t="s">
-        <v>139</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2003,19 +2032,19 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>200</v>
+        <v>131</v>
       </c>
       <c r="E8" t="s">
-        <v>207</v>
+        <v>136</v>
       </c>
       <c r="F8" t="s">
-        <v>208</v>
+        <v>137</v>
       </c>
       <c r="G8" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="H8" t="s">
-        <v>210</v>
+        <v>139</v>
       </c>
       <c r="I8" t="s">
         <v>61</v>
@@ -2038,13 +2067,13 @@
         <v>207</v>
       </c>
       <c r="F9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="I9" t="s">
         <v>61</v>
@@ -2061,50 +2090,50 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
+        <v>200</v>
+      </c>
+      <c r="E10" t="s">
+        <v>207</v>
+      </c>
+      <c r="F10" t="s">
+        <v>211</v>
+      </c>
+      <c r="G10" t="s">
+        <v>212</v>
+      </c>
+      <c r="H10" t="s">
+        <v>213</v>
+      </c>
+      <c r="I10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F10" t="s">
-        <v>141</v>
-      </c>
-      <c r="G10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" t="s">
-        <v>145</v>
-      </c>
-      <c r="I10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>131</v>
-      </c>
-      <c r="E11" t="s">
-        <v>140</v>
-      </c>
-      <c r="F11" t="s">
-        <v>141</v>
-      </c>
-      <c r="G11" t="s">
-        <v>142</v>
-      </c>
-      <c r="H11" t="s">
-        <v>143</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="E11" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2128,7 +2157,7 @@
         <v>141</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="H12" t="s">
         <v>145</v>
@@ -2154,13 +2183,13 @@
         <v>140</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>141</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>142</v>
       </c>
       <c r="H13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I13" t="s">
         <v>144</v>
@@ -2177,19 +2206,19 @@
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="E14" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="F14" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="G14" t="s">
-        <v>167</v>
+        <v>63</v>
       </c>
       <c r="H14" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="I14" t="s">
         <v>144</v>
@@ -2206,19 +2235,19 @@
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="E15" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="F15" t="s">
-        <v>169</v>
+        <v>63</v>
       </c>
       <c r="G15" t="s">
-        <v>170</v>
+        <v>63</v>
       </c>
       <c r="H15" t="s">
-        <v>171</v>
+        <v>145</v>
       </c>
       <c r="I15" t="s">
         <v>144</v>
@@ -2241,13 +2270,13 @@
         <v>165</v>
       </c>
       <c r="F16" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G16" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="H16" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="I16" t="s">
         <v>144</v>
@@ -2261,22 +2290,22 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>233</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>234</v>
+        <v>156</v>
       </c>
       <c r="E17" t="s">
-        <v>235</v>
+        <v>165</v>
       </c>
       <c r="F17" t="s">
-        <v>236</v>
+        <v>169</v>
       </c>
       <c r="G17" t="s">
-        <v>237</v>
+        <v>170</v>
       </c>
       <c r="H17" t="s">
-        <v>238</v>
+        <v>171</v>
       </c>
       <c r="I17" t="s">
         <v>144</v>
@@ -2290,22 +2319,22 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>233</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>239</v>
+        <v>156</v>
       </c>
       <c r="E18" t="s">
-        <v>240</v>
+        <v>165</v>
       </c>
       <c r="F18" t="s">
-        <v>241</v>
+        <v>172</v>
       </c>
       <c r="G18" t="s">
-        <v>242</v>
+        <v>173</v>
       </c>
       <c r="H18" t="s">
-        <v>243</v>
+        <v>174</v>
       </c>
       <c r="I18" t="s">
         <v>144</v>
@@ -2319,22 +2348,22 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>294</v>
+        <v>233</v>
       </c>
       <c r="D19" t="s">
-        <v>295</v>
+        <v>234</v>
       </c>
       <c r="E19" t="s">
-        <v>296</v>
+        <v>235</v>
       </c>
       <c r="F19" t="s">
-        <v>297</v>
+        <v>236</v>
       </c>
       <c r="G19" t="s">
-        <v>63</v>
+        <v>237</v>
       </c>
       <c r="H19" t="s">
-        <v>298</v>
+        <v>238</v>
       </c>
       <c r="I19" t="s">
         <v>144</v>
@@ -2351,22 +2380,22 @@
         <v>233</v>
       </c>
       <c r="D20" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="E20" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="F20" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>242</v>
       </c>
       <c r="H20" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="I20" t="s">
-        <v>253</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -2377,25 +2406,25 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>294</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>295</v>
       </c>
       <c r="E21" t="s">
-        <v>87</v>
+        <v>296</v>
       </c>
       <c r="F21" t="s">
-        <v>88</v>
+        <v>297</v>
       </c>
       <c r="G21" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="H21" t="s">
-        <v>90</v>
+        <v>298</v>
       </c>
       <c r="I21" t="s">
-        <v>91</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -2406,54 +2435,54 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>233</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>249</v>
       </c>
       <c r="E22" t="s">
-        <v>52</v>
+        <v>250</v>
       </c>
       <c r="F22" t="s">
-        <v>53</v>
+        <v>251</v>
       </c>
       <c r="G22" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="H22" t="s">
-        <v>55</v>
+        <v>252</v>
       </c>
       <c r="I22" t="s">
-        <v>56</v>
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>56</v>
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" t="s">
+        <v>89</v>
+      </c>
+      <c r="H23" t="s">
+        <v>90</v>
+      </c>
+      <c r="I23" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -2467,50 +2496,50 @@
         <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G24" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H24" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I24" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F25" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" t="s">
-        <v>70</v>
-      </c>
-      <c r="H25" t="s">
-        <v>71</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="F25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2525,50 +2554,50 @@
         <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F26" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G26" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="I26" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F27" s="1" t="s">
+      <c r="A27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="I27" s="1" t="s">
+      <c r="H27" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2583,50 +2612,50 @@
         <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E28" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="F28" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G28" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="H28" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="I28" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" t="s">
-        <v>72</v>
-      </c>
-      <c r="E29" t="s">
-        <v>77</v>
-      </c>
-      <c r="F29" t="s">
-        <v>78</v>
-      </c>
-      <c r="G29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" t="s">
-        <v>81</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="A29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2644,16 +2673,16 @@
         <v>72</v>
       </c>
       <c r="E30" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F30" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="H30" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="I30" t="s">
         <v>56</v>
@@ -2670,50 +2699,50 @@
         <v>11</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>175</v>
+        <v>72</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>176</v>
+        <v>73</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>177</v>
+        <v>63</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>178</v>
+        <v>63</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>180</v>
+        <v>301</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="I32" s="1" t="s">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" t="s">
+        <v>78</v>
+      </c>
+      <c r="G32" t="s">
+        <v>79</v>
+      </c>
+      <c r="H32" t="s">
+        <v>80</v>
+      </c>
+      <c r="I32" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2728,19 +2757,19 @@
         <v>11</v>
       </c>
       <c r="D33" t="s">
-        <v>175</v>
+        <v>72</v>
       </c>
       <c r="E33" t="s">
-        <v>176</v>
+        <v>77</v>
       </c>
       <c r="F33" t="s">
-        <v>177</v>
+        <v>78</v>
       </c>
       <c r="G33" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="H33" t="s">
-        <v>182</v>
+        <v>81</v>
       </c>
       <c r="I33" t="s">
         <v>56</v>
@@ -2757,108 +2786,108 @@
         <v>11</v>
       </c>
       <c r="D34" t="s">
-        <v>183</v>
+        <v>72</v>
       </c>
       <c r="E34" t="s">
-        <v>184</v>
+        <v>77</v>
       </c>
       <c r="F34" t="s">
-        <v>185</v>
+        <v>23</v>
       </c>
       <c r="G34" t="s">
-        <v>186</v>
+        <v>15</v>
       </c>
       <c r="H34" t="s">
-        <v>187</v>
+        <v>81</v>
       </c>
       <c r="I34" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" t="s">
-        <v>183</v>
-      </c>
-      <c r="E35" t="s">
-        <v>188</v>
-      </c>
-      <c r="F35" t="s">
-        <v>189</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="A35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>175</v>
+      </c>
+      <c r="E37" t="s">
+        <v>176</v>
+      </c>
+      <c r="F37" t="s">
+        <v>177</v>
+      </c>
+      <c r="G37" t="s">
         <v>63</v>
       </c>
-      <c r="H35" t="s">
-        <v>190</v>
-      </c>
-      <c r="I35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" t="s">
-        <v>183</v>
-      </c>
-      <c r="E36" t="s">
-        <v>188</v>
-      </c>
-      <c r="F36" t="s">
-        <v>191</v>
-      </c>
-      <c r="G36" t="s">
-        <v>63</v>
-      </c>
-      <c r="H36" t="s">
-        <v>192</v>
-      </c>
-      <c r="I36" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="I37" s="1" t="s">
+      <c r="H37" t="s">
+        <v>182</v>
+      </c>
+      <c r="I37" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2873,19 +2902,19 @@
         <v>11</v>
       </c>
       <c r="D38" t="s">
-        <v>214</v>
+        <v>183</v>
       </c>
       <c r="E38" t="s">
-        <v>215</v>
+        <v>184</v>
       </c>
       <c r="F38" t="s">
-        <v>216</v>
+        <v>185</v>
       </c>
       <c r="G38" t="s">
-        <v>63</v>
+        <v>186</v>
       </c>
       <c r="H38" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="I38" t="s">
         <v>56</v>
@@ -2899,22 +2928,22 @@
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>233</v>
+        <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>244</v>
+        <v>183</v>
       </c>
       <c r="E39" t="s">
-        <v>245</v>
+        <v>188</v>
       </c>
       <c r="F39" t="s">
-        <v>246</v>
+        <v>189</v>
       </c>
       <c r="G39" t="s">
-        <v>247</v>
+        <v>63</v>
       </c>
       <c r="H39" t="s">
-        <v>248</v>
+        <v>190</v>
       </c>
       <c r="I39" t="s">
         <v>56</v>
@@ -2931,51 +2960,51 @@
         <v>11</v>
       </c>
       <c r="D40" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="E40" t="s">
-        <v>27</v>
+        <v>188</v>
       </c>
       <c r="F40" t="s">
-        <v>23</v>
+        <v>191</v>
       </c>
       <c r="G40" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="H40" t="s">
-        <v>28</v>
+        <v>192</v>
       </c>
       <c r="I40" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" t="s">
-        <v>21</v>
-      </c>
-      <c r="E41" t="s">
-        <v>22</v>
-      </c>
-      <c r="F41" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" t="s">
-        <v>15</v>
-      </c>
-      <c r="H41" t="s">
-        <v>24</v>
-      </c>
-      <c r="I41" t="s">
-        <v>25</v>
+      <c r="A41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -2986,25 +3015,25 @@
         <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>227</v>
+        <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="E42" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="F42" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="G42" t="s">
         <v>63</v>
       </c>
       <c r="H42" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="I42" t="s">
-        <v>232</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -3015,25 +3044,25 @@
         <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="D43" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="E43" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="F43" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="G43" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="H43" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="I43" t="s">
-        <v>232</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -3044,25 +3073,25 @@
         <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>254</v>
+        <v>11</v>
       </c>
       <c r="D44" t="s">
-        <v>255</v>
+        <v>26</v>
       </c>
       <c r="E44" t="s">
-        <v>260</v>
+        <v>27</v>
       </c>
       <c r="F44" t="s">
-        <v>261</v>
+        <v>23</v>
       </c>
       <c r="G44" t="s">
-        <v>262</v>
+        <v>15</v>
       </c>
       <c r="H44" t="s">
-        <v>263</v>
+        <v>28</v>
       </c>
       <c r="I44" t="s">
-        <v>232</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -3073,25 +3102,25 @@
         <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>254</v>
+        <v>11</v>
       </c>
       <c r="D45" t="s">
-        <v>264</v>
+        <v>21</v>
       </c>
       <c r="E45" t="s">
-        <v>265</v>
+        <v>22</v>
       </c>
       <c r="F45" t="s">
-        <v>266</v>
+        <v>23</v>
       </c>
       <c r="G45" t="s">
-        <v>267</v>
+        <v>15</v>
       </c>
       <c r="H45" t="s">
-        <v>268</v>
+        <v>24</v>
       </c>
       <c r="I45" t="s">
-        <v>232</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -3102,22 +3131,22 @@
         <v>10</v>
       </c>
       <c r="C46" t="s">
-        <v>254</v>
+        <v>227</v>
       </c>
       <c r="D46" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="E46" t="s">
-        <v>265</v>
+        <v>229</v>
       </c>
       <c r="F46" t="s">
-        <v>269</v>
+        <v>230</v>
       </c>
       <c r="G46" t="s">
-        <v>270</v>
+        <v>63</v>
       </c>
       <c r="H46" t="s">
-        <v>271</v>
+        <v>231</v>
       </c>
       <c r="I46" t="s">
         <v>232</v>
@@ -3134,19 +3163,19 @@
         <v>254</v>
       </c>
       <c r="D47" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="E47" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="F47" t="s">
-        <v>23</v>
+        <v>257</v>
       </c>
       <c r="G47" t="s">
-        <v>15</v>
+        <v>258</v>
       </c>
       <c r="H47" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="I47" t="s">
         <v>232</v>
@@ -3163,19 +3192,19 @@
         <v>254</v>
       </c>
       <c r="D48" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="E48" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="F48" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="G48" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="H48" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="I48" t="s">
         <v>232</v>
@@ -3195,16 +3224,16 @@
         <v>264</v>
       </c>
       <c r="E49" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="F49" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="G49" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="H49" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="I49" t="s">
         <v>232</v>
@@ -3224,16 +3253,16 @@
         <v>264</v>
       </c>
       <c r="E50" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="F50" t="s">
-        <v>63</v>
+        <v>269</v>
       </c>
       <c r="G50" t="s">
-        <v>63</v>
+        <v>270</v>
       </c>
       <c r="H50" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="I50" t="s">
         <v>232</v>
@@ -3253,16 +3282,16 @@
         <v>264</v>
       </c>
       <c r="E51" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="F51" t="s">
-        <v>281</v>
+        <v>23</v>
       </c>
       <c r="G51" t="s">
-        <v>282</v>
+        <v>15</v>
       </c>
       <c r="H51" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="I51" t="s">
         <v>232</v>
@@ -3282,16 +3311,16 @@
         <v>264</v>
       </c>
       <c r="E52" t="s">
-        <v>63</v>
+        <v>272</v>
       </c>
       <c r="F52" t="s">
-        <v>23</v>
+        <v>273</v>
       </c>
       <c r="G52" t="s">
-        <v>15</v>
+        <v>274</v>
       </c>
       <c r="H52" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="I52" t="s">
         <v>232</v>
@@ -3311,16 +3340,16 @@
         <v>264</v>
       </c>
       <c r="E53" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="F53" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="G53" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="H53" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="I53" t="s">
         <v>232</v>
@@ -3340,16 +3369,16 @@
         <v>264</v>
       </c>
       <c r="E54" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="F54" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="G54" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="H54" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="I54" t="s">
         <v>232</v>
@@ -3369,16 +3398,16 @@
         <v>264</v>
       </c>
       <c r="E55" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F55" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="G55" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="H55" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="I55" t="s">
         <v>232</v>
@@ -3395,7 +3424,7 @@
         <v>254</v>
       </c>
       <c r="D56" t="s">
-        <v>63</v>
+        <v>264</v>
       </c>
       <c r="E56" t="s">
         <v>63</v>
@@ -3407,7 +3436,7 @@
         <v>15</v>
       </c>
       <c r="H56" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I56" t="s">
         <v>232</v>
@@ -3421,25 +3450,25 @@
         <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
+        <v>254</v>
       </c>
       <c r="D57" t="s">
-        <v>44</v>
+        <v>264</v>
       </c>
       <c r="E57" t="s">
-        <v>45</v>
+        <v>284</v>
       </c>
       <c r="F57" t="s">
-        <v>46</v>
+        <v>285</v>
       </c>
       <c r="G57" t="s">
-        <v>47</v>
+        <v>286</v>
       </c>
       <c r="H57" t="s">
-        <v>48</v>
+        <v>287</v>
       </c>
       <c r="I57" t="s">
-        <v>49</v>
+        <v>232</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -3450,13 +3479,13 @@
         <v>10</v>
       </c>
       <c r="C58" t="s">
-        <v>11</v>
+        <v>254</v>
       </c>
       <c r="D58" t="s">
-        <v>44</v>
+        <v>264</v>
       </c>
       <c r="E58" t="s">
-        <v>45</v>
+        <v>284</v>
       </c>
       <c r="F58" t="s">
         <v>23</v>
@@ -3465,10 +3494,10 @@
         <v>15</v>
       </c>
       <c r="H58" t="s">
-        <v>50</v>
+        <v>291</v>
       </c>
       <c r="I58" t="s">
-        <v>49</v>
+        <v>232</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -3479,25 +3508,25 @@
         <v>10</v>
       </c>
       <c r="C59" t="s">
-        <v>11</v>
+        <v>254</v>
       </c>
       <c r="D59" t="s">
-        <v>12</v>
+        <v>264</v>
       </c>
       <c r="E59" t="s">
-        <v>13</v>
+        <v>284</v>
       </c>
       <c r="F59" t="s">
-        <v>14</v>
+        <v>288</v>
       </c>
       <c r="G59" t="s">
-        <v>15</v>
+        <v>289</v>
       </c>
       <c r="H59" t="s">
-        <v>16</v>
+        <v>290</v>
       </c>
       <c r="I59" t="s">
-        <v>17</v>
+        <v>232</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
@@ -3508,25 +3537,25 @@
         <v>10</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>254</v>
       </c>
       <c r="D60" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="E60" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="F60" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G60" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H60" t="s">
-        <v>20</v>
+        <v>293</v>
       </c>
       <c r="I60" t="s">
-        <v>17</v>
+        <v>232</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -3540,22 +3569,22 @@
         <v>11</v>
       </c>
       <c r="D61" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="E61" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F61" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="G61" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="H61" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="I61" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
@@ -3569,22 +3598,22 @@
         <v>11</v>
       </c>
       <c r="D62" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="E62" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F62" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="G62" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H62" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="I62" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
@@ -3598,19 +3627,19 @@
         <v>11</v>
       </c>
       <c r="D63" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E63" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F63" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="G63" t="s">
         <v>15</v>
       </c>
       <c r="H63" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="I63" t="s">
         <v>17</v>
@@ -3627,19 +3656,19 @@
         <v>11</v>
       </c>
       <c r="D64" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E64" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F64" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="G64" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H64" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I64" t="s">
         <v>17</v>
@@ -3662,13 +3691,13 @@
         <v>30</v>
       </c>
       <c r="F65" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G65" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="H65" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I65" t="s">
         <v>17</v>
@@ -3691,44 +3720,44 @@
         <v>30</v>
       </c>
       <c r="F66" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G66" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="H66" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="I66" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I67" s="1" t="s">
+      <c r="A67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" t="s">
+        <v>26</v>
+      </c>
+      <c r="E67" t="s">
+        <v>30</v>
+      </c>
+      <c r="F67" t="s">
+        <v>34</v>
+      </c>
+      <c r="G67" t="s">
+        <v>15</v>
+      </c>
+      <c r="H67" t="s">
+        <v>37</v>
+      </c>
+      <c r="I67" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3743,19 +3772,19 @@
         <v>11</v>
       </c>
       <c r="D68" t="s">
-        <v>92</v>
+        <v>26</v>
       </c>
       <c r="E68" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="F68" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="G68" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="H68" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="I68" t="s">
         <v>17</v>
@@ -3772,19 +3801,19 @@
         <v>11</v>
       </c>
       <c r="D69" t="s">
-        <v>104</v>
+        <v>26</v>
       </c>
       <c r="E69" t="s">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="F69" t="s">
-        <v>106</v>
+        <v>38</v>
       </c>
       <c r="G69" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="H69" t="s">
-        <v>108</v>
+        <v>40</v>
       </c>
       <c r="I69" t="s">
         <v>17</v>
@@ -3801,50 +3830,50 @@
         <v>11</v>
       </c>
       <c r="D70" t="s">
-        <v>104</v>
+        <v>26</v>
       </c>
       <c r="E70" t="s">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="F70" t="s">
-        <v>106</v>
+        <v>41</v>
       </c>
       <c r="G70" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="H70" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="I70" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>9</v>
-      </c>
-      <c r="B71" t="s">
-        <v>10</v>
-      </c>
-      <c r="C71" t="s">
-        <v>11</v>
-      </c>
-      <c r="D71" t="s">
-        <v>104</v>
-      </c>
-      <c r="E71" t="s">
-        <v>105</v>
-      </c>
-      <c r="F71" t="s">
-        <v>23</v>
-      </c>
-      <c r="G71" t="s">
-        <v>15</v>
-      </c>
-      <c r="H71" t="s">
-        <v>109</v>
-      </c>
-      <c r="I71" t="s">
+      <c r="A71" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I71" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3859,19 +3888,19 @@
         <v>11</v>
       </c>
       <c r="D72" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="E72" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F72" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G72" t="s">
-        <v>111</v>
+        <v>63</v>
       </c>
       <c r="H72" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="I72" t="s">
         <v>17</v>
@@ -3894,13 +3923,13 @@
         <v>105</v>
       </c>
       <c r="F73" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G73" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="H73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I73" t="s">
         <v>17</v>
@@ -3923,10 +3952,10 @@
         <v>105</v>
       </c>
       <c r="F74" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="G74" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="H74" t="s">
         <v>109</v>
@@ -3952,13 +3981,13 @@
         <v>105</v>
       </c>
       <c r="F75" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
       <c r="G75" t="s">
-        <v>116</v>
+        <v>15</v>
       </c>
       <c r="H75" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="I75" t="s">
         <v>17</v>
@@ -3981,13 +4010,13 @@
         <v>105</v>
       </c>
       <c r="F76" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="G76" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="H76" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="I76" t="s">
         <v>17</v>
@@ -4010,13 +4039,13 @@
         <v>105</v>
       </c>
       <c r="F77" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G77" t="s">
-        <v>122</v>
+        <v>63</v>
       </c>
       <c r="H77" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="I77" t="s">
         <v>17</v>
@@ -4039,7 +4068,7 @@
         <v>105</v>
       </c>
       <c r="F78" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="G78" t="s">
         <v>63</v>
@@ -4068,13 +4097,13 @@
         <v>105</v>
       </c>
       <c r="F79" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G79" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="H79" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="I79" t="s">
         <v>17</v>
@@ -4097,13 +4126,13 @@
         <v>105</v>
       </c>
       <c r="F80" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G80" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H80" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="I80" t="s">
         <v>17</v>
@@ -4126,13 +4155,13 @@
         <v>105</v>
       </c>
       <c r="F81" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="G81" t="s">
-        <v>15</v>
+        <v>122</v>
       </c>
       <c r="H81" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="I81" t="s">
         <v>17</v>
@@ -4155,7 +4184,7 @@
         <v>105</v>
       </c>
       <c r="F82" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="G82" t="s">
         <v>63</v>
@@ -4181,16 +4210,16 @@
         <v>104</v>
       </c>
       <c r="E83" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="F83" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G83" t="s">
-        <v>129</v>
+        <v>15</v>
       </c>
       <c r="H83" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="I83" t="s">
         <v>17</v>
@@ -4207,19 +4236,19 @@
         <v>11</v>
       </c>
       <c r="D84" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="E84" t="s">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="F84" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="G84" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="H84" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="I84" t="s">
         <v>17</v>
@@ -4236,19 +4265,19 @@
         <v>11</v>
       </c>
       <c r="D85" t="s">
-        <v>200</v>
+        <v>104</v>
       </c>
       <c r="E85" t="s">
-        <v>201</v>
+        <v>105</v>
       </c>
       <c r="F85" t="s">
-        <v>202</v>
+        <v>63</v>
       </c>
       <c r="G85" t="s">
-        <v>203</v>
+        <v>15</v>
       </c>
       <c r="H85" t="s">
-        <v>204</v>
+        <v>109</v>
       </c>
       <c r="I85" t="s">
         <v>17</v>
@@ -4265,80 +4294,80 @@
         <v>11</v>
       </c>
       <c r="D86" t="s">
-        <v>200</v>
+        <v>104</v>
       </c>
       <c r="E86" t="s">
-        <v>201</v>
+        <v>105</v>
       </c>
       <c r="F86" t="s">
-        <v>202</v>
+        <v>63</v>
       </c>
       <c r="G86" t="s">
-        <v>205</v>
+        <v>63</v>
       </c>
       <c r="H86" t="s">
-        <v>206</v>
+        <v>109</v>
       </c>
       <c r="I86" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I87" s="1" t="s">
-        <v>299</v>
+      <c r="A87" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" t="s">
+        <v>10</v>
+      </c>
+      <c r="C87" t="s">
+        <v>11</v>
+      </c>
+      <c r="D87" t="s">
+        <v>104</v>
+      </c>
+      <c r="E87" t="s">
+        <v>127</v>
+      </c>
+      <c r="F87" t="s">
+        <v>128</v>
+      </c>
+      <c r="G87" t="s">
+        <v>129</v>
+      </c>
+      <c r="H87" t="s">
+        <v>130</v>
+      </c>
+      <c r="I87" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I88" s="1" t="s">
-        <v>103</v>
+      <c r="A88" t="s">
+        <v>9</v>
+      </c>
+      <c r="B88" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" t="s">
+        <v>131</v>
+      </c>
+      <c r="E88" t="s">
+        <v>148</v>
+      </c>
+      <c r="F88" t="s">
+        <v>149</v>
+      </c>
+      <c r="G88" t="s">
+        <v>150</v>
+      </c>
+      <c r="H88" t="s">
+        <v>151</v>
+      </c>
+      <c r="I88" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
@@ -4352,108 +4381,108 @@
         <v>11</v>
       </c>
       <c r="D89" t="s">
-        <v>131</v>
+        <v>200</v>
       </c>
       <c r="E89" t="s">
-        <v>132</v>
+        <v>201</v>
       </c>
       <c r="F89" t="s">
-        <v>133</v>
+        <v>202</v>
       </c>
       <c r="G89" t="s">
-        <v>134</v>
+        <v>203</v>
       </c>
       <c r="H89" t="s">
-        <v>135</v>
+        <v>204</v>
       </c>
       <c r="I89" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F90" s="1" t="s">
+      <c r="A90" t="s">
+        <v>9</v>
+      </c>
+      <c r="B90" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90" t="s">
+        <v>200</v>
+      </c>
+      <c r="E90" t="s">
+        <v>201</v>
+      </c>
+      <c r="F90" t="s">
+        <v>202</v>
+      </c>
+      <c r="G90" t="s">
+        <v>205</v>
+      </c>
+      <c r="H90" t="s">
+        <v>206</v>
+      </c>
+      <c r="I90" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F91" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G90" s="1" t="s">
+      <c r="G91" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H90" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I90" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>9</v>
-      </c>
-      <c r="B91" t="s">
-        <v>10</v>
-      </c>
-      <c r="C91" t="s">
-        <v>11</v>
-      </c>
-      <c r="D91" t="s">
-        <v>156</v>
-      </c>
-      <c r="E91" t="s">
-        <v>157</v>
-      </c>
-      <c r="F91" t="s">
-        <v>158</v>
-      </c>
-      <c r="G91" t="s">
-        <v>159</v>
-      </c>
-      <c r="H91" t="s">
-        <v>160</v>
-      </c>
-      <c r="I91" t="s">
-        <v>103</v>
+      <c r="H91" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>9</v>
-      </c>
-      <c r="B92" t="s">
-        <v>10</v>
-      </c>
-      <c r="C92" t="s">
-        <v>11</v>
-      </c>
-      <c r="D92" t="s">
-        <v>156</v>
-      </c>
-      <c r="E92" t="s">
-        <v>157</v>
-      </c>
-      <c r="F92" t="s">
-        <v>158</v>
-      </c>
-      <c r="G92" t="s">
-        <v>161</v>
-      </c>
-      <c r="H92" t="s">
-        <v>162</v>
-      </c>
-      <c r="I92" t="s">
+      <c r="A92" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I92" s="1" t="s">
         <v>103</v>
       </c>
     </row>
@@ -4468,50 +4497,50 @@
         <v>11</v>
       </c>
       <c r="D93" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="E93" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="F93" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="G93" t="s">
-        <v>15</v>
+        <v>134</v>
       </c>
       <c r="H93" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="I93" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>9</v>
-      </c>
-      <c r="B94" t="s">
-        <v>10</v>
-      </c>
-      <c r="C94" t="s">
-        <v>11</v>
-      </c>
-      <c r="D94" t="s">
-        <v>218</v>
-      </c>
-      <c r="E94" t="s">
-        <v>223</v>
-      </c>
-      <c r="F94" t="s">
-        <v>224</v>
-      </c>
-      <c r="G94" t="s">
-        <v>225</v>
-      </c>
-      <c r="H94" t="s">
-        <v>226</v>
-      </c>
-      <c r="I94" t="s">
+      <c r="A94" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I94" s="1" t="s">
         <v>103</v>
       </c>
     </row>
@@ -4526,33 +4555,149 @@
         <v>11</v>
       </c>
       <c r="D95" t="s">
+        <v>156</v>
+      </c>
+      <c r="E95" t="s">
+        <v>157</v>
+      </c>
+      <c r="F95" t="s">
+        <v>158</v>
+      </c>
+      <c r="G95" t="s">
+        <v>159</v>
+      </c>
+      <c r="H95" t="s">
+        <v>160</v>
+      </c>
+      <c r="I95" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>9</v>
+      </c>
+      <c r="B96" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96" t="s">
+        <v>11</v>
+      </c>
+      <c r="D96" t="s">
+        <v>156</v>
+      </c>
+      <c r="E96" t="s">
+        <v>157</v>
+      </c>
+      <c r="F96" t="s">
+        <v>158</v>
+      </c>
+      <c r="G96" t="s">
+        <v>161</v>
+      </c>
+      <c r="H96" t="s">
+        <v>162</v>
+      </c>
+      <c r="I96" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>9</v>
+      </c>
+      <c r="B97" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97" t="s">
+        <v>11</v>
+      </c>
+      <c r="D97" t="s">
+        <v>156</v>
+      </c>
+      <c r="E97" t="s">
+        <v>157</v>
+      </c>
+      <c r="F97" t="s">
+        <v>163</v>
+      </c>
+      <c r="G97" t="s">
+        <v>15</v>
+      </c>
+      <c r="H97" t="s">
+        <v>164</v>
+      </c>
+      <c r="I97" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>9</v>
+      </c>
+      <c r="B98" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D98" t="s">
+        <v>218</v>
+      </c>
+      <c r="E98" t="s">
+        <v>223</v>
+      </c>
+      <c r="F98" t="s">
+        <v>224</v>
+      </c>
+      <c r="G98" t="s">
+        <v>225</v>
+      </c>
+      <c r="H98" t="s">
+        <v>226</v>
+      </c>
+      <c r="I98" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>9</v>
+      </c>
+      <c r="B99" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D99" t="s">
         <v>183</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E99" t="s">
         <v>196</v>
       </c>
-      <c r="F95" t="s">
+      <c r="F99" t="s">
         <v>197</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G99" t="s">
         <v>198</v>
       </c>
-      <c r="H95" t="s">
+      <c r="H99" t="s">
         <v>199</v>
       </c>
-      <c r="I95" t="s">
+      <c r="I99" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I95">
-    <sortCondition ref="I2:I95"/>
-    <sortCondition ref="B2:B95"/>
-    <sortCondition ref="C2:C95"/>
-    <sortCondition ref="D2:D95"/>
-    <sortCondition ref="E2:E95"/>
-    <sortCondition ref="F2:F95"/>
-    <sortCondition ref="G2:G95"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I99">
+    <sortCondition ref="I2:I99"/>
+    <sortCondition ref="B2:B99"/>
+    <sortCondition ref="C2:C99"/>
+    <sortCondition ref="D2:D99"/>
+    <sortCondition ref="E2:E99"/>
+    <sortCondition ref="F2:F99"/>
+    <sortCondition ref="G2:G99"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>